<commit_message>
#17 - Validacao de nome de proprietario e responsavel
</commit_message>
<xml_diff>
--- a/documents/recadastramento/layouts/Layout_Retorno_Cadastro.xlsx
+++ b/documents/recadastramento/layouts/Layout_Retorno_Cadastro.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="22202"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24560" windowHeight="15620" tabRatio="657" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24800" windowHeight="15620" tabRatio="657" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Cabeçalho" sheetId="17" r:id="rId1"/>
@@ -15,7 +15,7 @@
     <sheet name="Medidor" sheetId="4" r:id="rId6"/>
     <sheet name="Anormalidade Imovel" sheetId="16" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="124519" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -1501,8 +1501,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:XFD56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C20" sqref="A20:XFD36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1819,7 +1819,7 @@
       </c>
       <c r="F20" s="9"/>
       <c r="XFD20">
-        <f>SUM(C20:XFC20)</f>
+        <f t="shared" ref="XFD20:XFD36" si="1">SUM(C20:XFC20)</f>
         <v>186</v>
       </c>
     </row>
@@ -1837,7 +1837,7 @@
       <c r="E21" s="8"/>
       <c r="F21" s="9"/>
       <c r="XFD21">
-        <f>SUM(C21:XFC21)</f>
+        <f t="shared" si="1"/>
         <v>236</v>
       </c>
     </row>
@@ -1859,7 +1859,7 @@
         <v>93</v>
       </c>
       <c r="XFD22">
-        <f>SUM(C22:XFC22)</f>
+        <f t="shared" si="1"/>
         <v>237</v>
       </c>
     </row>
@@ -1877,7 +1877,7 @@
       <c r="E23" s="8"/>
       <c r="F23" s="16"/>
       <c r="XFD23">
-        <f>SUM(C23:XFC23)</f>
+        <f t="shared" si="1"/>
         <v>251</v>
       </c>
     </row>
@@ -1895,7 +1895,7 @@
       <c r="E24" s="8"/>
       <c r="F24" s="16"/>
       <c r="XFD24">
-        <f>SUM(C24:XFC24)</f>
+        <f t="shared" si="1"/>
         <v>260</v>
       </c>
     </row>
@@ -1915,7 +1915,7 @@
       </c>
       <c r="F25" s="16"/>
       <c r="XFD25">
-        <f>SUM(C25:XFC25)</f>
+        <f t="shared" si="1"/>
         <v>262</v>
       </c>
     </row>
@@ -1937,7 +1937,7 @@
         <v>95</v>
       </c>
       <c r="XFD26">
-        <f>SUM(C26:XFC26)</f>
+        <f t="shared" si="1"/>
         <v>263</v>
       </c>
     </row>
@@ -1955,7 +1955,7 @@
       <c r="E27" s="8"/>
       <c r="F27" s="9"/>
       <c r="XFD27">
-        <f>SUM(C27:XFC27)</f>
+        <f t="shared" si="1"/>
         <v>273</v>
       </c>
     </row>
@@ -1973,7 +1973,7 @@
       <c r="E28" s="8"/>
       <c r="F28" s="9"/>
       <c r="XFD28">
-        <f>SUM(C28:XFC28)</f>
+        <f t="shared" si="1"/>
         <v>283</v>
       </c>
     </row>
@@ -1991,7 +1991,7 @@
       <c r="E29" s="8"/>
       <c r="F29" s="9"/>
       <c r="XFD29">
-        <f>SUM(C29:XFC29)</f>
+        <f t="shared" si="1"/>
         <v>313</v>
       </c>
     </row>
@@ -2009,7 +2009,7 @@
       <c r="E30" s="8"/>
       <c r="F30" s="9"/>
       <c r="XFD30">
-        <f>SUM(C30:XFC30)</f>
+        <f t="shared" si="1"/>
         <v>315</v>
       </c>
     </row>
@@ -2027,7 +2027,7 @@
       <c r="E31" s="8"/>
       <c r="F31" s="9"/>
       <c r="XFD31">
-        <f>SUM(C31:XFC31)</f>
+        <f t="shared" si="1"/>
         <v>355</v>
       </c>
     </row>
@@ -2045,7 +2045,7 @@
       <c r="E32" s="8"/>
       <c r="F32" s="9"/>
       <c r="XFD32">
-        <f>SUM(C32:XFC32)</f>
+        <f t="shared" si="1"/>
         <v>360</v>
       </c>
     </row>
@@ -2063,7 +2063,7 @@
       <c r="E33" s="8"/>
       <c r="F33" s="9"/>
       <c r="XFD33">
-        <f>SUM(C33:XFC33)</f>
+        <f t="shared" si="1"/>
         <v>385</v>
       </c>
     </row>
@@ -2081,7 +2081,7 @@
       <c r="E34" s="8"/>
       <c r="F34" s="9"/>
       <c r="XFD34">
-        <f>SUM(C34:XFC34)</f>
+        <f t="shared" si="1"/>
         <v>405</v>
       </c>
     </row>
@@ -2099,7 +2099,7 @@
       <c r="E35" s="8"/>
       <c r="F35" s="9"/>
       <c r="XFD35">
-        <f>SUM(C35:XFC35)</f>
+        <f t="shared" si="1"/>
         <v>413</v>
       </c>
     </row>
@@ -2117,7 +2117,7 @@
       <c r="E36" s="8"/>
       <c r="F36" s="9"/>
       <c r="XFD36">
-        <f>SUM(C36:XFC36)</f>
+        <f t="shared" si="1"/>
         <v>428</v>
       </c>
     </row>
@@ -2434,7 +2434,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
#17 - Validacao de ramo de atividade
</commit_message>
<xml_diff>
--- a/documents/recadastramento/layouts/Layout_Retorno_Cadastro.xlsx
+++ b/documents/recadastramento/layouts/Layout_Retorno_Cadastro.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="22202"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24800" windowHeight="15620" tabRatio="657" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24600" windowHeight="15620" tabRatio="657" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Cabeçalho" sheetId="17" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="142">
   <si>
     <t>Nome do Campo</t>
   </si>
@@ -1501,8 +1501,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:XFD56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2434,8 +2434,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H42"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -3130,26 +3130,27 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:E5"/>
+  <dimension ref="B1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="24.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.33203125" customWidth="1"/>
-    <col min="5" max="5" width="48" customWidth="1"/>
+    <col min="4" max="4" width="8.33203125" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" customWidth="1"/>
+    <col min="6" max="6" width="48" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="24" thickBot="1">
+    <row r="1" spans="2:6" ht="24" thickBot="1">
       <c r="B1" s="3" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="2" spans="2:5" ht="15" thickBot="1">
+    <row r="2" spans="2:6" ht="15" thickBot="1">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -3157,43 +3158,57 @@
         <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="1"/>
-    </row>
-    <row r="3" spans="2:5" ht="15" thickBot="1">
+      <c r="F2" s="1"/>
+    </row>
+    <row r="3" spans="2:6" ht="15" thickBot="1">
       <c r="B3" s="7" t="s">
         <v>127</v>
       </c>
       <c r="C3" s="8">
         <v>2</v>
       </c>
-      <c r="D3" s="38"/>
-      <c r="E3" s="14" t="s">
+      <c r="D3" s="8">
+        <v>1</v>
+      </c>
+      <c r="E3" s="38"/>
+      <c r="F3" s="14" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="4" spans="2:5">
+    <row r="4" spans="2:6">
       <c r="B4" s="24" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="22">
         <v>9</v>
       </c>
-      <c r="D4" s="47" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="25"/>
-    </row>
-    <row r="5" spans="2:5" ht="15" thickBot="1">
+      <c r="D4" s="5">
+        <f>SUM(C3,D3)</f>
+        <v>3</v>
+      </c>
+      <c r="E4" s="47" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="25"/>
+    </row>
+    <row r="5" spans="2:6" ht="15" thickBot="1">
       <c r="B5" s="17" t="s">
         <v>92</v>
       </c>
       <c r="C5" s="18">
         <v>3</v>
       </c>
-      <c r="D5" s="19"/>
-      <c r="E5" s="20"/>
+      <c r="D5" s="5">
+        <f>SUM(C4,D4)</f>
+        <v>12</v>
+      </c>
+      <c r="E5" s="19"/>
+      <c r="F5" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
Alteração para validar linha tipo 03 apenas quando código for maior que 0
</commit_message>
<xml_diff>
--- a/documents/recadastramento/layouts/Layout_Retorno_Cadastro.xlsx
+++ b/documents/recadastramento/layouts/Layout_Retorno_Cadastro.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="1" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="657" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="6" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="657" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Cabeçalho" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="142">
   <si>
     <t>linha tipo 00</t>
   </si>
@@ -251,7 +251,7 @@
     <t>Longitude</t>
   </si>
   <si>
-    <t>Data </t>
+    <t>Data</t>
   </si>
   <si>
     <t>Date</t>
@@ -272,7 +272,7 @@
     <t>inscricao</t>
   </si>
   <si>
-    <t>Se tamanho 16, será adicionado valor "0" antes do  valor rota </t>
+    <t>Se tamanho 16, será adicionado valor "0" antes do  valor rota</t>
   </si>
   <si>
     <t>face</t>
@@ -434,13 +434,7 @@
     <t>tipo_caixa_protecao</t>
   </si>
   <si>
-    <t>Latitude </t>
-  </si>
-  <si>
     <t>Longetude</t>
-  </si>
-  <si>
-    <t>Data</t>
   </si>
   <si>
     <t>linha tipo 06</t>
@@ -601,7 +595,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
@@ -663,10 +657,6 @@
       <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="8" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -758,7 +748,7 @@
   <dimension ref="B2:F11"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="F4" activeCellId="0" pane="topLeft" sqref="F4"/>
+      <selection activeCell="F4" activeCellId="1" pane="topLeft" sqref="D5:D13 F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.3"/>
@@ -937,8 +927,8 @@
   </sheetPr>
   <dimension ref="B1:F65536"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A4" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="D1" activeCellId="0" pane="topLeft" sqref="D1"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A4" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="D1" activeCellId="1" pane="topLeft" sqref="D5:D13 D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.3"/>
@@ -1819,7 +1809,7 @@
   <dimension ref="B1:H65536"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A25" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="F18" activeCellId="0" pane="topLeft" sqref="F18"/>
+      <selection activeCell="F18" activeCellId="1" pane="topLeft" sqref="D5:D13 F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.3"/>
@@ -2529,23 +2519,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:E7"/>
+  <dimension ref="B1:F7"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="E5" activeCellId="0" pane="topLeft" sqref="E5"/>
+      <selection activeCell="D4" activeCellId="1" pane="topLeft" sqref="D5:D13 D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="13.3"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.83400809716599"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.165991902834"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.33198380566802"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.331983805668"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="33.8502024291498"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.83400809716599"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="9.07692307692308"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="33.8502024291498"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.83400809716599"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="24" outlineLevel="0" r="1">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="21.7" outlineLevel="0" r="1">
       <c r="B1" s="1" t="s">
         <v>117</v>
       </c>
@@ -2558,9 +2548,12 @@
         <v>2</v>
       </c>
       <c r="D2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2571,8 +2564,11 @@
       <c r="C3" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="7" t="s">
+      <c r="D3" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" s="6"/>
+      <c r="F3" s="7" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2583,10 +2579,14 @@
       <c r="C4" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="D4" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="4"/>
+      <c r="D4" s="5" t="n">
+        <f aca="false">SUM(C3,D3)</f>
+        <v>3</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="4"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="5">
       <c r="B5" s="4" t="s">
@@ -2595,24 +2595,29 @@
       <c r="C5" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="D5" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="13" t="s">
+      <c r="D5" s="5" t="n">
+        <f aca="false">SUM(C4,D4)</f>
+        <v>12</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="13" t="s">
         <v>50</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="45.5" outlineLevel="0" r="7" s="16">
-      <c r="B7" s="17" t="s">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="45.5" outlineLevel="0" r="7">
+      <c r="B7" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B7:F7"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.511805555555555" right="0.511805555555555" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
@@ -2629,22 +2634,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:G10"/>
+  <dimension ref="B1:H10"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="E14" activeCellId="0" pane="topLeft" sqref="E14"/>
+      <selection activeCell="D4" activeCellId="1" pane="topLeft" sqref="D5:D13 D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="13.3"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.83400809716599"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.004048582996"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="8.83400809716599"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.8623481781376"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.83400809716599"/>
+    <col collapsed="false" hidden="false" max="5" min="3" style="0" width="8.83400809716599"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="31.8623481781376"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.83400809716599"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="24" outlineLevel="0" r="1">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="21.7" outlineLevel="0" r="1">
       <c r="B1" s="1" t="s">
         <v>120</v>
       </c>
@@ -2657,9 +2662,12 @@
         <v>2</v>
       </c>
       <c r="D2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2670,8 +2678,11 @@
       <c r="C3" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="7" t="s">
+      <c r="D3" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" s="6"/>
+      <c r="F3" s="7" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2682,10 +2693,14 @@
       <c r="C4" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="D4" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="13"/>
+      <c r="D4" s="5" t="n">
+        <f aca="false">SUM(C3,D3)</f>
+        <v>3</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="13"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="5">
       <c r="B5" s="4" t="s">
@@ -2694,10 +2709,14 @@
       <c r="C5" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="18" t="s">
+      <c r="D5" s="5" t="n">
+        <f aca="false">SUM(C4,D4)</f>
+        <v>12</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="17" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2708,10 +2727,14 @@
       <c r="C6" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="D6" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" s="18"/>
+      <c r="D6" s="5" t="n">
+        <f aca="false">SUM(C5,D5)</f>
+        <v>14</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="17"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="7">
       <c r="B7" s="4" t="s">
@@ -2720,10 +2743,14 @@
       <c r="C7" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="D7" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" s="18"/>
+      <c r="D7" s="5" t="n">
+        <f aca="false">SUM(C6,D6)</f>
+        <v>16</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="17"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="8">
       <c r="B8" s="4" t="s">
@@ -2732,10 +2759,14 @@
       <c r="C8" s="5" t="n">
         <v>20</v>
       </c>
-      <c r="D8" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="4"/>
+      <c r="D8" s="5" t="n">
+        <f aca="false">SUM(C7,D7)</f>
+        <v>18</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="4"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="9">
       <c r="B9" s="4" t="s">
@@ -2744,11 +2775,15 @@
       <c r="C9" s="5" t="n">
         <v>20</v>
       </c>
-      <c r="D9" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" s="4"/>
-      <c r="G9" s="15"/>
+      <c r="D9" s="5" t="n">
+        <f aca="false">SUM(C8,D8)</f>
+        <v>38</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="4"/>
+      <c r="H9" s="15"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="10">
       <c r="B10" s="4" t="s">
@@ -2757,10 +2792,14 @@
       <c r="C10" s="6" t="n">
         <v>26</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="5" t="n">
+        <f aca="false">SUM(C9,D9)</f>
+        <v>58</v>
+      </c>
+      <c r="E10" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2778,23 +2817,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:E12"/>
+  <dimension ref="B1:F12"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="E9" activeCellId="0" pane="topLeft" sqref="E9"/>
+      <selection activeCell="D4" activeCellId="1" pane="topLeft" sqref="D5:D13 D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="13.3"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.83400809716599"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.502024291498"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.83400809716599"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.5060728744939"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="60"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.83400809716599"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="9.90688259109312"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="32.1943319838057"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.83400809716599"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="24" outlineLevel="0" r="1">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="21.7" outlineLevel="0" r="1">
       <c r="B1" s="1" t="s">
         <v>124</v>
       </c>
@@ -2807,9 +2846,12 @@
         <v>2</v>
       </c>
       <c r="D2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2820,8 +2862,11 @@
       <c r="C3" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="7" t="s">
+      <c r="D3" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" s="6"/>
+      <c r="F3" s="7" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2832,10 +2877,14 @@
       <c r="C4" s="6" t="n">
         <v>9</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="13"/>
+      <c r="D4" s="6" t="n">
+        <f aca="false">SUM(C3,D3)</f>
+        <v>3</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="13"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="5">
       <c r="B5" s="4" t="s">
@@ -2844,10 +2893,14 @@
       <c r="C5" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="4" t="s">
+      <c r="D5" s="6" t="n">
+        <f aca="false">SUM(C4,D4)</f>
+        <v>12</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="4" t="s">
         <v>126</v>
       </c>
     </row>
@@ -2858,10 +2911,14 @@
       <c r="C6" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="D6" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="4"/>
+      <c r="D6" s="6" t="n">
+        <f aca="false">SUM(C5,D5)</f>
+        <v>13</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="4"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="7">
       <c r="B7" s="4" t="s">
@@ -2870,10 +2927,14 @@
       <c r="C7" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="D7" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" s="13" t="s">
+      <c r="D7" s="6" t="n">
+        <f aca="false">SUM(C6,D6)</f>
+        <v>23</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="13" t="s">
         <v>129</v>
       </c>
     </row>
@@ -2884,10 +2945,14 @@
       <c r="C8" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="6" t="n">
+        <f aca="false">SUM(C7,D7)</f>
+        <v>25</v>
+      </c>
+      <c r="E8" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="E8" s="13" t="s">
+      <c r="F8" s="13" t="s">
         <v>129</v>
       </c>
     </row>
@@ -2898,48 +2963,64 @@
       <c r="C9" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="D9" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9" s="13" t="s">
+      <c r="D9" s="6" t="n">
+        <f aca="false">SUM(C8,D8)</f>
+        <v>27</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="13" t="s">
         <v>50</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="10">
       <c r="B10" s="4" t="s">
-        <v>133</v>
+        <v>74</v>
       </c>
       <c r="C10" s="5" t="n">
         <v>20</v>
       </c>
-      <c r="D10" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" s="4"/>
+      <c r="D10" s="6" t="n">
+        <f aca="false">SUM(C9,D9)</f>
+        <v>29</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="4"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="11">
       <c r="B11" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C11" s="5" t="n">
         <v>20</v>
       </c>
-      <c r="D11" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11" s="4"/>
+      <c r="D11" s="6" t="n">
+        <f aca="false">SUM(C10,D10)</f>
+        <v>49</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="4"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="12">
       <c r="B12" s="4" t="s">
-        <v>135</v>
+        <v>76</v>
       </c>
       <c r="C12" s="5" t="n">
         <v>26</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="6" t="n">
+        <f aca="false">SUM(C11,D11)</f>
+        <v>69</v>
+      </c>
+      <c r="E12" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2957,24 +3038,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B2:E13"/>
+  <dimension ref="B2:F13"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B5" activeCellId="0" pane="topLeft" sqref="B5"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="D5" activeCellId="0" pane="topLeft" sqref="D5:D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="13.3"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.83400809716599"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="8.83400809716599"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="44.9919028340081"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.83400809716599"/>
+    <col collapsed="false" hidden="false" max="5" min="3" style="0" width="8.83400809716599"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="45.6113360323887"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.83400809716599"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="24" outlineLevel="0" r="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="21.7" outlineLevel="0" r="2">
       <c r="B2" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="3">
@@ -2985,9 +3066,12 @@
         <v>2</v>
       </c>
       <c r="D3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="F3" s="3" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2998,8 +3082,11 @@
       <c r="C4" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="D4" s="6"/>
-      <c r="E4" s="7" t="s">
+      <c r="D4" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" s="6"/>
+      <c r="F4" s="7" t="s">
         <v>7</v>
       </c>
     </row>
@@ -3010,60 +3097,80 @@
       <c r="C5" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="4"/>
+      <c r="D5" s="5" t="n">
+        <f aca="false">SUM(C4,D4)</f>
+        <v>3</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="4"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="6">
       <c r="B6" s="4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C6" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="D6" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>138</v>
+      <c r="D6" s="5" t="n">
+        <f aca="false">SUM(C5,D5)</f>
+        <v>12</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>136</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="7">
       <c r="B7" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C7" s="5" t="n">
         <v>200</v>
       </c>
-      <c r="D7" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="4"/>
+      <c r="D7" s="5" t="n">
+        <f aca="false">SUM(C6,D6)</f>
+        <v>15</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="4"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="8">
       <c r="B8" s="4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C8" s="5" t="n">
         <v>30</v>
       </c>
-      <c r="D8" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="4"/>
+      <c r="D8" s="5" t="n">
+        <f aca="false">SUM(C7,D7)</f>
+        <v>215</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="4"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="9">
       <c r="B9" s="4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C9" s="5" t="n">
         <v>30</v>
       </c>
-      <c r="D9" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" s="4"/>
+      <c r="D9" s="5" t="n">
+        <f aca="false">SUM(C8,D8)</f>
+        <v>245</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="4"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="10">
       <c r="B10" s="4" t="s">
@@ -3072,10 +3179,14 @@
       <c r="C10" s="5" t="n">
         <v>20</v>
       </c>
-      <c r="D10" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" s="4"/>
+      <c r="D10" s="5" t="n">
+        <f aca="false">SUM(C9,D9)</f>
+        <v>275</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="4"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="11">
       <c r="B11" s="4" t="s">
@@ -3084,35 +3195,47 @@
       <c r="C11" s="5" t="n">
         <v>20</v>
       </c>
-      <c r="D11" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11" s="4"/>
+      <c r="D11" s="5" t="n">
+        <f aca="false">SUM(C10,D10)</f>
+        <v>295</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="4"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="12">
       <c r="B12" s="4" t="s">
-        <v>135</v>
+        <v>76</v>
       </c>
       <c r="C12" s="5" t="n">
         <v>26</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="5" t="n">
+        <f aca="false">SUM(C11,D11)</f>
+        <v>315</v>
+      </c>
+      <c r="E12" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="13">
       <c r="B13" s="7" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C13" s="9" t="n">
         <v>20</v>
       </c>
-      <c r="D13" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>143</v>
+      <c r="D13" s="5" t="n">
+        <f aca="false">SUM(C12,D12)</f>
+        <v>341</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>141</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Alterando layouts de Recadastramento
</commit_message>
<xml_diff>
--- a/documents/recadastramento/layouts/Layout_Retorno_Cadastro.xlsx
+++ b/documents/recadastramento/layouts/Layout_Retorno_Cadastro.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="6" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="657" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="2" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="657" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Cabeçalho" sheetId="1" state="visible" r:id="rId2"/>
@@ -13,7 +13,7 @@
     <sheet name="Imovel" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Ramo de Atividade do Imovel" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="Servicos" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="Medidor" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="Hidrômetro" sheetId="6" state="visible" r:id="rId7"/>
     <sheet name="Anormalidade Imovel" sheetId="7" state="visible" r:id="rId8"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="148">
   <si>
     <t>linha tipo 00</t>
   </si>
@@ -44,36 +44,39 @@
     <t>linha tipo</t>
   </si>
   <si>
+    <t>Identificação do tipo da linha</t>
+  </si>
+  <si>
+    <t>grupo</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>localidade</t>
+  </si>
+  <si>
+    <t>setor</t>
+  </si>
+  <si>
+    <t>rota</t>
+  </si>
+  <si>
+    <t>Ano/Mês Referência</t>
+  </si>
+  <si>
+    <t>id_rota</t>
+  </si>
+  <si>
+    <t>versao_do aplicativo de cadastro</t>
+  </si>
+  <si>
+    <t>linha tipo 01</t>
+  </si>
+  <si>
     <t>utilizado para identificar o tipo da linha</t>
   </si>
   <si>
-    <t>grupo</t>
-  </si>
-  <si>
-    <t>String</t>
-  </si>
-  <si>
-    <t>localidade</t>
-  </si>
-  <si>
-    <t>setor</t>
-  </si>
-  <si>
-    <t>rota</t>
-  </si>
-  <si>
-    <t>Ano/Mês Referência</t>
-  </si>
-  <si>
-    <t>id_rota</t>
-  </si>
-  <si>
-    <t>versao_do aplicativo de cadastro</t>
-  </si>
-  <si>
-    <t>linha tipo 01</t>
-  </si>
-  <si>
     <t>matricula</t>
   </si>
   <si>
@@ -83,6 +86,9 @@
     <t>gerencia</t>
   </si>
   <si>
+    <t>Ex: Metropolitana, Regional</t>
+  </si>
+  <si>
     <t>tipo_endereço_proprietario</t>
   </si>
   <si>
@@ -134,6 +140,9 @@
     <t>telefone_usuario</t>
   </si>
   <si>
+    <t>DDD + Telefone (ex: 9132220000)</t>
+  </si>
+  <si>
     <t>celular_usuario</t>
   </si>
   <si>
@@ -296,6 +305,29 @@
     <t>tipo_logradouro_imovel</t>
   </si>
   <si>
+    <r>
+      <t xml:space="preserve">Relacionado a linha tipo 09 do arquivo de rota (</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <color rgb="FFFF0000"/>
+        <sz val="11"/>
+      </rPr>
+      <t xml:space="preserve">NÃO PODE SER ZERO OU NULO</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <color rgb="FF000000"/>
+        <sz val="11"/>
+      </rPr>
+      <t xml:space="preserve">)</t>
+    </r>
+  </si>
+  <si>
     <t>logradouro_imovel</t>
   </si>
   <si>
@@ -320,9 +352,6 @@
     <t>sub_categoria_residencial_1</t>
   </si>
   <si>
-    <t>Número de economias nesta subcategoria</t>
-  </si>
-  <si>
     <t>sub_categoria_residencial_2</t>
   </si>
   <si>
@@ -371,7 +400,7 @@
     <t>tipo_fonte_abastecimento</t>
   </si>
   <si>
-    <t>Relacionado à linha tipo 12 do arquivo de rota.</t>
+    <t>Relacionado à linha tipo 13 do arquivo de rota</t>
   </si>
   <si>
     <t>linha tipo 03</t>
@@ -401,12 +430,81 @@
     <t>tipo_ligacao_agua</t>
   </si>
   <si>
+    <r>
+      <t xml:space="preserve">Relacionado a linha tipo 10 do arquivo de rota (</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <color rgb="FFFF0000"/>
+        <sz val="11"/>
+      </rPr>
+      <t xml:space="preserve">NÃO PODE SER ZERO OU NULO</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <color rgb="FF000000"/>
+        <sz val="11"/>
+      </rPr>
+      <t xml:space="preserve">)</t>
+    </r>
+  </si>
+  <si>
     <t>tipo_ligacao_esgoto</t>
   </si>
   <si>
+    <r>
+      <t xml:space="preserve">Relacionado a linha tipo 11 do arquivo de rota (</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <color rgb="FFFF0000"/>
+        <sz val="11"/>
+      </rPr>
+      <t xml:space="preserve">NÃO PODE SER ZERO OU NULO</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <color rgb="FF000000"/>
+        <sz val="11"/>
+      </rPr>
+      <t xml:space="preserve">)</t>
+    </r>
+  </si>
+  <si>
     <t>local_instalacao_ramal</t>
   </si>
   <si>
+    <r>
+      <t xml:space="preserve">Relacionado a linha tipo 15 do arquivo de rota (</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <color rgb="FFFF0000"/>
+        <sz val="11"/>
+      </rPr>
+      <t xml:space="preserve">NÃO PODE SER ZERO OU NULO</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <color rgb="FF000000"/>
+        <sz val="11"/>
+      </rPr>
+      <t xml:space="preserve">)</t>
+    </r>
+  </si>
+  <si>
     <t>linha tipo 05</t>
   </si>
   <si>
@@ -422,28 +520,88 @@
     <t>marca</t>
   </si>
   <si>
-    <t>Informação desconsiderada</t>
+    <r>
+      <t xml:space="preserve">Relacionado a linha tipo 14 do arquivo de rota (</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <color rgb="FFFF0000"/>
+        <sz val="11"/>
+      </rPr>
+      <t xml:space="preserve">NÃO PODE SER ZERO OU NULO</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <color rgb="FF000000"/>
+        <sz val="11"/>
+      </rPr>
+      <t xml:space="preserve">)</t>
+    </r>
   </si>
   <si>
     <t>capacidade</t>
   </si>
   <si>
-    <t>Double</t>
+    <r>
+      <t xml:space="preserve">Relacionado a linha tipo 16 do arquivo de rota (</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <color rgb="FFFF0000"/>
+        <sz val="11"/>
+      </rPr>
+      <t xml:space="preserve">NÃO PODE SER ZERO OU NULO</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <color rgb="FF000000"/>
+        <sz val="11"/>
+      </rPr>
+      <t xml:space="preserve">)</t>
+    </r>
   </si>
   <si>
     <t>tipo_caixa_protecao</t>
   </si>
   <si>
+    <r>
+      <t xml:space="preserve">Relacionado a linha tipo 12 do arquivo de rota (</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <color rgb="FFFF0000"/>
+        <sz val="11"/>
+      </rPr>
+      <t xml:space="preserve">NÃO PODE SER ZERO OU NULO</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <color rgb="FF000000"/>
+        <sz val="11"/>
+      </rPr>
+      <t xml:space="preserve">)</t>
+    </r>
+  </si>
+  <si>
     <t>Longetude</t>
   </si>
   <si>
     <t>linha tipo 06</t>
   </si>
   <si>
-    <t>codigo de Anormalidade</t>
-  </si>
-  <si>
-    <t>Ocorrência de Cadastro</t>
+    <t>codigo de anormalidade</t>
   </si>
   <si>
     <t>Comentário</t>
@@ -468,7 +626,7 @@
   <numFmts count="1">
     <numFmt formatCode="GENERAL" numFmtId="164"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="12">
     <font>
       <name val="Calibri"/>
       <charset val="1"/>
@@ -529,6 +687,18 @@
     <font>
       <name val="Calibri"/>
       <charset val="1"/>
+      <family val="2"/>
+      <color rgb="FFFF0000"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color rgb="FF000000"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
       <family val="2"/>
       <color rgb="FFFF0000"/>
       <sz val="11"/>
@@ -595,7 +765,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="30">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
@@ -656,16 +826,64 @@
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="3" fontId="5" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="3" fontId="5" numFmtId="164" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="false" borderId="1" fillId="3" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="3" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="3" fontId="10" numFmtId="164" xfId="0">
+      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="8" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="3" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="3" fontId="6" numFmtId="164" xfId="0">
       <alignment horizontal="justify" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="3" fontId="9" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="3" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="3" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="false" borderId="1" fillId="3" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="3" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="3" fontId="10" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
   </cellXfs>
@@ -748,7 +966,7 @@
   <dimension ref="B2:F11"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="F4" activeCellId="1" pane="topLeft" sqref="D5:D13 F4"/>
+      <selection activeCell="F5" activeCellId="0" pane="topLeft" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.3"/>
@@ -927,8 +1145,8 @@
   </sheetPr>
   <dimension ref="B1:F65536"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A4" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="D1" activeCellId="1" pane="topLeft" sqref="D5:D13 D1"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A22" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="F30" activeCellId="0" pane="topLeft" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.3"/>
@@ -976,12 +1194,12 @@
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="7" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="4">
       <c r="B4" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C4" s="5" t="n">
         <v>9</v>
@@ -991,13 +1209,13 @@
         <v>3</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F4" s="4"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="5">
       <c r="B5" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C5" s="5" t="n">
         <v>25</v>
@@ -1009,11 +1227,13 @@
       <c r="E5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="4"/>
+      <c r="F5" s="4" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="6">
       <c r="B6" s="4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C6" s="5" t="n">
         <v>1</v>
@@ -1023,15 +1243,15 @@
         <v>37</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="7">
       <c r="B7" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C7" s="5" t="n">
         <v>1</v>
@@ -1041,15 +1261,15 @@
         <v>38</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="8">
       <c r="B8" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C8" s="5" t="n">
         <v>1</v>
@@ -1059,15 +1279,15 @@
         <v>39</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="9">
       <c r="B9" s="7" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C9" s="9" t="n">
         <v>1</v>
@@ -1077,15 +1297,15 @@
         <v>40</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="10">
       <c r="B10" s="10" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C10" s="5" t="n">
         <v>9</v>
@@ -1095,13 +1315,13 @@
         <v>41</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F10" s="4"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="11">
       <c r="B11" s="4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C11" s="5" t="n">
         <v>50</v>
@@ -1110,12 +1330,14 @@
         <f aca="false">SUM(C10,D10)</f>
         <v>50</v>
       </c>
-      <c r="E11" s="5"/>
+      <c r="E11" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="F11" s="4"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="12">
       <c r="B12" s="4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C12" s="5" t="n">
         <v>1</v>
@@ -1125,15 +1347,15 @@
         <v>100</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="13">
       <c r="B13" s="4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C13" s="5" t="n">
         <v>14</v>
@@ -1142,12 +1364,14 @@
         <f aca="false">SUM(C12,D12)</f>
         <v>101</v>
       </c>
-      <c r="E13" s="5"/>
+      <c r="E13" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="F13" s="4"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="14">
       <c r="B14" s="4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C14" s="5" t="n">
         <v>9</v>
@@ -1156,12 +1380,14 @@
         <f aca="false">SUM(C13,D13)</f>
         <v>115</v>
       </c>
-      <c r="E14" s="5"/>
+      <c r="E14" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="F14" s="4"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="15">
       <c r="B15" s="4" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C15" s="5" t="n">
         <v>2</v>
@@ -1177,7 +1403,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="16">
       <c r="B16" s="4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C16" s="5" t="n">
         <v>1</v>
@@ -1187,15 +1413,15 @@
         <v>126</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="17">
       <c r="B17" s="4" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C17" s="5" t="n">
         <v>10</v>
@@ -1204,12 +1430,16 @@
         <f aca="false">SUM(C16,D16)</f>
         <v>127</v>
       </c>
-      <c r="E17" s="5"/>
-      <c r="F17" s="4"/>
+      <c r="E17" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="18">
       <c r="B18" s="4" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C18" s="5" t="n">
         <v>10</v>
@@ -1218,12 +1448,16 @@
         <f aca="false">SUM(C17,D17)</f>
         <v>137</v>
       </c>
-      <c r="E18" s="5"/>
-      <c r="F18" s="4"/>
+      <c r="E18" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="19">
       <c r="B19" s="4" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C19" s="5" t="n">
         <v>30</v>
@@ -1232,12 +1466,14 @@
         <f aca="false">SUM(C18,D18)</f>
         <v>147</v>
       </c>
-      <c r="E19" s="5"/>
+      <c r="E19" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="F19" s="4"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="20">
       <c r="B20" s="10" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C20" s="5" t="n">
         <v>9</v>
@@ -1247,13 +1483,13 @@
         <v>177</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F20" s="4"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="21">
       <c r="B21" s="4" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C21" s="5" t="n">
         <v>50</v>
@@ -1262,12 +1498,14 @@
         <f aca="false">SUM(C20,D20)</f>
         <v>186</v>
       </c>
-      <c r="E21" s="5"/>
+      <c r="E21" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="F21" s="4"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="22">
       <c r="B22" s="4" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C22" s="5" t="n">
         <v>1</v>
@@ -1277,15 +1515,15 @@
         <v>236</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F22" s="11" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="23">
       <c r="B23" s="4" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C23" s="5" t="n">
         <v>14</v>
@@ -1294,12 +1532,14 @@
         <f aca="false">SUM(C22,D22)</f>
         <v>237</v>
       </c>
-      <c r="E23" s="5"/>
+      <c r="E23" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="F23" s="12"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="24">
       <c r="B24" s="4" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C24" s="5" t="n">
         <v>9</v>
@@ -1308,12 +1548,14 @@
         <f aca="false">SUM(C23,D23)</f>
         <v>251</v>
       </c>
-      <c r="E24" s="5"/>
+      <c r="E24" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="F24" s="12"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="25">
       <c r="B25" s="4" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C25" s="5" t="n">
         <v>2</v>
@@ -1329,7 +1571,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="26">
       <c r="B26" s="4" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C26" s="5" t="n">
         <v>1</v>
@@ -1339,15 +1581,15 @@
         <v>262</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F26" s="11" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="27">
       <c r="B27" s="4" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C27" s="5" t="n">
         <v>10</v>
@@ -1356,12 +1598,16 @@
         <f aca="false">SUM(C26,D26)</f>
         <v>263</v>
       </c>
-      <c r="E27" s="5"/>
-      <c r="F27" s="4"/>
+      <c r="E27" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="28">
       <c r="B28" s="4" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C28" s="5" t="n">
         <v>10</v>
@@ -1370,12 +1616,16 @@
         <f aca="false">SUM(C27,D27)</f>
         <v>273</v>
       </c>
-      <c r="E28" s="5"/>
-      <c r="F28" s="4"/>
+      <c r="E28" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="29">
       <c r="B29" s="4" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C29" s="5" t="n">
         <v>30</v>
@@ -1384,12 +1634,14 @@
         <f aca="false">SUM(C28,D28)</f>
         <v>283</v>
       </c>
-      <c r="E29" s="5"/>
+      <c r="E29" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="F29" s="4"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="30">
       <c r="B30" s="4" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C30" s="5" t="n">
         <v>2</v>
@@ -1398,14 +1650,16 @@
         <f aca="false">SUM(C29,D29)</f>
         <v>313</v>
       </c>
-      <c r="E30" s="5"/>
+      <c r="E30" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="F30" s="13" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="31">
       <c r="B31" s="4" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C31" s="5" t="n">
         <v>40</v>
@@ -1414,12 +1668,14 @@
         <f aca="false">SUM(C30,D30)</f>
         <v>315</v>
       </c>
-      <c r="E31" s="5"/>
+      <c r="E31" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="F31" s="4"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="32">
       <c r="B32" s="4" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C32" s="5" t="n">
         <v>5</v>
@@ -1428,12 +1684,14 @@
         <f aca="false">SUM(C31,D31)</f>
         <v>355</v>
       </c>
-      <c r="E32" s="5"/>
+      <c r="E32" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="F32" s="4"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="33">
       <c r="B33" s="4" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="C33" s="5" t="n">
         <v>25</v>
@@ -1442,12 +1700,14 @@
         <f aca="false">SUM(C32,D32)</f>
         <v>360</v>
       </c>
-      <c r="E33" s="5"/>
+      <c r="E33" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="F33" s="4"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="34">
       <c r="B34" s="4" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C34" s="5" t="n">
         <v>20</v>
@@ -1456,12 +1716,14 @@
         <f aca="false">SUM(C33,D33)</f>
         <v>385</v>
       </c>
-      <c r="E34" s="5"/>
+      <c r="E34" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="F34" s="4"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="35">
       <c r="B35" s="4" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C35" s="5" t="n">
         <v>8</v>
@@ -1470,12 +1732,14 @@
         <f aca="false">SUM(C34,D34)</f>
         <v>405</v>
       </c>
-      <c r="E35" s="5"/>
+      <c r="E35" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="F35" s="4"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="36">
       <c r="B36" s="4" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C36" s="5" t="n">
         <v>15</v>
@@ -1484,12 +1748,14 @@
         <f aca="false">SUM(C35,D35)</f>
         <v>413</v>
       </c>
-      <c r="E36" s="5"/>
+      <c r="E36" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="F36" s="4"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="37">
       <c r="B37" s="10" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C37" s="5" t="n">
         <v>9</v>
@@ -1499,13 +1765,13 @@
         <v>428</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F37" s="4"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="38">
       <c r="B38" s="4" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C38" s="5" t="n">
         <v>50</v>
@@ -1514,12 +1780,14 @@
         <f aca="false">SUM(C37,D37)</f>
         <v>437</v>
       </c>
-      <c r="E38" s="5"/>
+      <c r="E38" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="F38" s="4"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="39">
       <c r="B39" s="4" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="C39" s="5" t="n">
         <v>1</v>
@@ -1529,15 +1797,15 @@
         <v>487</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F39" s="11" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="40">
       <c r="B40" s="4" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C40" s="5" t="n">
         <v>14</v>
@@ -1546,12 +1814,14 @@
         <f aca="false">SUM(C39,D39)</f>
         <v>488</v>
       </c>
-      <c r="E40" s="5"/>
+      <c r="E40" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="F40" s="12"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="41">
       <c r="B41" s="4" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="C41" s="5" t="n">
         <v>9</v>
@@ -1560,12 +1830,14 @@
         <f aca="false">SUM(C40,D40)</f>
         <v>502</v>
       </c>
-      <c r="E41" s="5"/>
+      <c r="E41" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="F41" s="12"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="42">
       <c r="B42" s="4" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="C42" s="5" t="n">
         <v>2</v>
@@ -1581,7 +1853,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="43">
       <c r="B43" s="4" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C43" s="5" t="n">
         <v>1</v>
@@ -1591,15 +1863,15 @@
         <v>513</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F43" s="11" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="44">
       <c r="B44" s="4" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C44" s="5" t="n">
         <v>10</v>
@@ -1608,12 +1880,16 @@
         <f aca="false">SUM(C43,D43)</f>
         <v>514</v>
       </c>
-      <c r="E44" s="5"/>
-      <c r="F44" s="4"/>
+      <c r="E44" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F44" s="4" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="45">
       <c r="B45" s="4" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="C45" s="5" t="n">
         <v>10</v>
@@ -1622,12 +1898,16 @@
         <f aca="false">SUM(C44,D44)</f>
         <v>524</v>
       </c>
-      <c r="E45" s="5"/>
-      <c r="F45" s="4"/>
+      <c r="E45" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F45" s="4" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="46">
       <c r="B46" s="4" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="C46" s="5" t="n">
         <v>30</v>
@@ -1636,12 +1916,14 @@
         <f aca="false">SUM(C45,D45)</f>
         <v>534</v>
       </c>
-      <c r="E46" s="5"/>
+      <c r="E46" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="F46" s="4"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="47">
       <c r="B47" s="4" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C47" s="5" t="n">
         <v>2</v>
@@ -1650,14 +1932,16 @@
         <f aca="false">SUM(C46,D46)</f>
         <v>564</v>
       </c>
-      <c r="E47" s="5"/>
+      <c r="E47" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="F47" s="13" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="48">
       <c r="B48" s="4" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="C48" s="5" t="n">
         <v>40</v>
@@ -1666,12 +1950,14 @@
         <f aca="false">SUM(C47,D47)</f>
         <v>566</v>
       </c>
-      <c r="E48" s="5"/>
+      <c r="E48" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="F48" s="4"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="49">
       <c r="B49" s="4" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="C49" s="5" t="n">
         <v>5</v>
@@ -1680,12 +1966,14 @@
         <f aca="false">SUM(C48,D48)</f>
         <v>606</v>
       </c>
-      <c r="E49" s="5"/>
+      <c r="E49" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="F49" s="4"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="50">
       <c r="B50" s="4" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="C50" s="5" t="n">
         <v>25</v>
@@ -1694,12 +1982,14 @@
         <f aca="false">SUM(C49,D49)</f>
         <v>611</v>
       </c>
-      <c r="E50" s="5"/>
+      <c r="E50" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="F50" s="4"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="51">
       <c r="B51" s="4" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C51" s="5" t="n">
         <v>20</v>
@@ -1708,12 +1998,14 @@
         <f aca="false">SUM(C50,D50)</f>
         <v>636</v>
       </c>
-      <c r="E51" s="5"/>
+      <c r="E51" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="F51" s="4"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="52">
       <c r="B52" s="4" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C52" s="5" t="n">
         <v>8</v>
@@ -1722,12 +2014,14 @@
         <f aca="false">SUM(C51,D51)</f>
         <v>656</v>
       </c>
-      <c r="E52" s="5"/>
+      <c r="E52" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="F52" s="4"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="53">
       <c r="B53" s="4" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="C53" s="5" t="n">
         <v>15</v>
@@ -1736,12 +2030,14 @@
         <f aca="false">SUM(C52,D52)</f>
         <v>664</v>
       </c>
-      <c r="E53" s="5"/>
+      <c r="E53" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="F53" s="4"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="54">
       <c r="B54" s="4" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="C54" s="5" t="n">
         <v>20</v>
@@ -1757,7 +2053,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="55">
       <c r="B55" s="4" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="C55" s="5" t="n">
         <v>20</v>
@@ -1773,7 +2069,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="56">
       <c r="B56" s="4" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C56" s="6" t="n">
         <v>26</v>
@@ -1783,7 +2079,7 @@
         <v>719</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="F56" s="14"/>
     </row>
@@ -1808,8 +2104,8 @@
   </sheetPr>
   <dimension ref="B1:H65536"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A25" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="F18" activeCellId="1" pane="topLeft" sqref="D5:D13 F18"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A31" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="F40" activeCellId="0" pane="topLeft" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.3"/>
@@ -1818,13 +2114,13 @@
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.502024291498"/>
     <col collapsed="false" hidden="false" max="4" min="3" style="0" width="8.83400809716599"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="8" width="8.83400809716599"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="50.502024291498"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="40.0404858299595"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.83400809716599"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="21.7" outlineLevel="0" r="1">
       <c r="B1" s="1" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="2">
@@ -1855,13 +2151,13 @@
         <v>1</v>
       </c>
       <c r="E3" s="6"/>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="4">
       <c r="B4" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C4" s="5" t="n">
         <v>9</v>
@@ -1871,31 +2167,31 @@
         <v>3</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F4" s="4"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="5">
-      <c r="B5" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="C5" s="9" t="n">
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="31.2" outlineLevel="0" r="5" s="15">
+      <c r="B5" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="C5" s="17" t="n">
         <v>1</v>
       </c>
-      <c r="D5" s="5" t="n">
+      <c r="D5" s="18" t="n">
         <f aca="false">SUM(C4,D4)</f>
         <v>12</v>
       </c>
-      <c r="E5" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>80</v>
+      <c r="E5" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="16" t="s">
+        <v>83</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="6">
       <c r="B6" s="7" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C6" s="9" t="n">
         <v>30</v>
@@ -1907,20 +2203,22 @@
       <c r="E6" s="9"/>
       <c r="F6" s="7"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="7">
-      <c r="B7" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="C7" s="5" t="n">
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="31.2" outlineLevel="0" r="7" s="15">
+      <c r="B7" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="C7" s="18" t="n">
         <v>17</v>
       </c>
-      <c r="D7" s="5" t="n">
+      <c r="D7" s="18" t="n">
         <f aca="false">SUM(C6,D6)</f>
         <v>43</v>
       </c>
-      <c r="E7" s="5"/>
-      <c r="F7" s="4" t="s">
-        <v>83</v>
+      <c r="E7" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="19" t="s">
+        <v>86</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="8">
@@ -1934,12 +2232,14 @@
         <f aca="false">SUM(C7,D7)</f>
         <v>60</v>
       </c>
-      <c r="E8" s="5"/>
+      <c r="E8" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="F8" s="4"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="9">
       <c r="B9" s="4" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="C9" s="5" t="n">
         <v>2</v>
@@ -1948,12 +2248,14 @@
         <f aca="false">SUM(C8,D8)</f>
         <v>62</v>
       </c>
-      <c r="E9" s="5"/>
+      <c r="E9" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="F9" s="4"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="10">
       <c r="B10" s="4" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="C10" s="6" t="n">
         <v>8</v>
@@ -1963,13 +2265,13 @@
         <v>64</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F10" s="13"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="11">
       <c r="B11" s="4" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="C11" s="5" t="n">
         <v>31</v>
@@ -1978,12 +2280,14 @@
         <f aca="false">SUM(C10,D10)</f>
         <v>72</v>
       </c>
-      <c r="E11" s="9"/>
+      <c r="E11" s="9" t="s">
+        <v>9</v>
+      </c>
       <c r="F11" s="4"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="12">
       <c r="B12" s="4" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="C12" s="5" t="n">
         <v>20</v>
@@ -1992,12 +2296,14 @@
         <f aca="false">SUM(C11,D11)</f>
         <v>103</v>
       </c>
-      <c r="E12" s="9"/>
+      <c r="E12" s="9" t="s">
+        <v>9</v>
+      </c>
       <c r="F12" s="4"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="13">
       <c r="B13" s="4" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="C13" s="5" t="n">
         <v>5</v>
@@ -2007,13 +2313,13 @@
         <v>123</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F13" s="4"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="14">
       <c r="B14" s="4" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="C14" s="5" t="n">
         <v>5</v>
@@ -2023,31 +2329,31 @@
         <v>128</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F14" s="4"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="15">
-      <c r="B15" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="C15" s="5" t="n">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="31.2" outlineLevel="0" r="15">
+      <c r="B15" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="C15" s="18" t="n">
         <v>2</v>
       </c>
-      <c r="D15" s="5" t="n">
+      <c r="D15" s="18" t="n">
         <f aca="false">SUM(C14,D14)</f>
         <v>133</v>
       </c>
-      <c r="E15" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="F15" s="13" t="s">
-        <v>50</v>
+      <c r="E15" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="F15" s="20" t="s">
+        <v>94</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="16">
       <c r="B16" s="4" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="C16" s="5" t="n">
         <v>40</v>
@@ -2056,12 +2362,14 @@
         <f aca="false">SUM(C15,D15)</f>
         <v>135</v>
       </c>
-      <c r="E16" s="5"/>
+      <c r="E16" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="F16" s="4"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="17">
       <c r="B17" s="4" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="C17" s="5" t="n">
         <v>5</v>
@@ -2070,12 +2378,14 @@
         <f aca="false">SUM(C16,D16)</f>
         <v>175</v>
       </c>
-      <c r="E17" s="5"/>
+      <c r="E17" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="F17" s="4"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="18">
       <c r="B18" s="4" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="C18" s="5" t="n">
         <v>25</v>
@@ -2084,12 +2394,14 @@
         <f aca="false">SUM(C17,D17)</f>
         <v>180</v>
       </c>
-      <c r="E18" s="5"/>
+      <c r="E18" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="F18" s="4"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="19">
       <c r="B19" s="4" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="C19" s="5" t="n">
         <v>20</v>
@@ -2098,12 +2410,14 @@
         <f aca="false">SUM(C18,D18)</f>
         <v>205</v>
       </c>
-      <c r="E19" s="5"/>
+      <c r="E19" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="F19" s="4"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="20">
       <c r="B20" s="4" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="C20" s="5" t="n">
         <v>8</v>
@@ -2112,12 +2426,14 @@
         <f aca="false">SUM(C19,D19)</f>
         <v>225</v>
       </c>
-      <c r="E20" s="5"/>
+      <c r="E20" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="F20" s="4"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="21">
       <c r="B21" s="4" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="C21" s="5" t="n">
         <v>15</v>
@@ -2126,12 +2442,14 @@
         <f aca="false">SUM(C20,D20)</f>
         <v>233</v>
       </c>
-      <c r="E21" s="5"/>
+      <c r="E21" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="F21" s="4"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="22">
       <c r="B22" s="4" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="C22" s="5" t="n">
         <v>9</v>
@@ -2140,12 +2458,14 @@
         <f aca="false">SUM(C21,D21)</f>
         <v>248</v>
       </c>
-      <c r="E22" s="5"/>
+      <c r="E22" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="F22" s="4"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="23">
       <c r="B23" s="10" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="C23" s="5" t="n">
         <v>3</v>
@@ -2155,15 +2475,13 @@
         <v>257</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>99</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="F23" s="4"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="24">
       <c r="B24" s="4" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="C24" s="5" t="n">
         <v>3</v>
@@ -2173,15 +2491,13 @@
         <v>260</v>
       </c>
       <c r="E24" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>99</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="F24" s="4"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="25">
       <c r="B25" s="4" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="C25" s="5" t="n">
         <v>3</v>
@@ -2191,15 +2507,13 @@
         <v>263</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>99</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="F25" s="4"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="26">
       <c r="B26" s="4" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="C26" s="5" t="n">
         <v>3</v>
@@ -2209,15 +2523,13 @@
         <v>266</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="F26" s="4" t="s">
-        <v>99</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="F26" s="4"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="27">
       <c r="B27" s="10" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="C27" s="5" t="n">
         <v>3</v>
@@ -2227,15 +2539,13 @@
         <v>269</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>99</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="F27" s="4"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="28">
       <c r="B28" s="4" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="C28" s="5" t="n">
         <v>3</v>
@@ -2245,15 +2555,13 @@
         <v>272</v>
       </c>
       <c r="E28" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>99</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="F28" s="4"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="29">
       <c r="B29" s="4" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C29" s="5" t="n">
         <v>3</v>
@@ -2263,15 +2571,13 @@
         <v>275</v>
       </c>
       <c r="E29" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="F29" s="4" t="s">
-        <v>99</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="F29" s="4"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="30">
       <c r="B30" s="4" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="C30" s="5" t="n">
         <v>3</v>
@@ -2281,15 +2587,13 @@
         <v>278</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="F30" s="4" t="s">
-        <v>99</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="F30" s="4"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="31">
       <c r="B31" s="10" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="C31" s="5" t="n">
         <v>3</v>
@@ -2299,15 +2603,13 @@
         <v>281</v>
       </c>
       <c r="E31" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="F31" s="4" t="s">
-        <v>99</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="F31" s="4"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="32">
       <c r="B32" s="4" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="C32" s="5" t="n">
         <v>3</v>
@@ -2317,15 +2619,13 @@
         <v>284</v>
       </c>
       <c r="E32" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="F32" s="4" t="s">
-        <v>99</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="F32" s="4"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="33">
       <c r="B33" s="4" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="C33" s="5" t="n">
         <v>3</v>
@@ -2335,15 +2635,13 @@
         <v>287</v>
       </c>
       <c r="E33" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="F33" s="4" t="s">
-        <v>99</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="F33" s="4"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="34">
       <c r="B34" s="4" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="C34" s="5" t="n">
         <v>3</v>
@@ -2353,15 +2651,13 @@
         <v>290</v>
       </c>
       <c r="E34" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="F34" s="4" t="s">
-        <v>99</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="F34" s="4"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="35">
       <c r="B35" s="10" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="C35" s="5" t="n">
         <v>3</v>
@@ -2371,15 +2667,13 @@
         <v>293</v>
       </c>
       <c r="E35" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="F35" s="4" t="s">
-        <v>99</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="F35" s="4"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="36">
       <c r="B36" s="4" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C36" s="5" t="n">
         <v>3</v>
@@ -2389,15 +2683,13 @@
         <v>296</v>
       </c>
       <c r="E36" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="F36" s="4" t="s">
-        <v>99</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="F36" s="4"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="37">
       <c r="B37" s="4" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="C37" s="5" t="n">
         <v>3</v>
@@ -2407,15 +2699,13 @@
         <v>299</v>
       </c>
       <c r="E37" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="F37" s="4" t="s">
-        <v>99</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="F37" s="4"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="38">
       <c r="B38" s="4" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="C38" s="5" t="n">
         <v>3</v>
@@ -2425,16 +2715,14 @@
         <v>302</v>
       </c>
       <c r="E38" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="F38" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="H38" s="15"/>
+        <v>19</v>
+      </c>
+      <c r="F38" s="4"/>
+      <c r="H38" s="21"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="39">
       <c r="B39" s="4" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="C39" s="6" t="n">
         <v>2</v>
@@ -2444,15 +2732,15 @@
         <v>305</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="40">
       <c r="B40" s="4" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="C40" s="5" t="n">
         <v>20</v>
@@ -2468,7 +2756,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="41">
       <c r="B41" s="4" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="C41" s="5" t="n">
         <v>20</v>
@@ -2484,7 +2772,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="42">
       <c r="B42" s="4" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C42" s="6" t="n">
         <v>26</v>
@@ -2494,7 +2782,7 @@
         <v>347</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="F42" s="14"/>
     </row>
@@ -2522,7 +2810,7 @@
   <dimension ref="B1:F7"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="D4" activeCellId="1" pane="topLeft" sqref="D5:D13 D4"/>
+      <selection activeCell="F5" activeCellId="0" pane="topLeft" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.3"/>
@@ -2531,13 +2819,13 @@
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.165991902834"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.33198380566802"/>
     <col collapsed="false" hidden="false" max="5" min="4" style="0" width="9.07692307692308"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="33.8502024291498"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="40.5546558704453"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.83400809716599"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="21.7" outlineLevel="0" r="1">
       <c r="B1" s="1" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="2">
@@ -2574,7 +2862,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="4">
       <c r="B4" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C4" s="5" t="n">
         <v>9</v>
@@ -2584,36 +2872,36 @@
         <v>3</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F4" s="4"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="5">
-      <c r="B5" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="C5" s="5" t="n">
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="30.55" outlineLevel="0" r="5" s="22">
+      <c r="B5" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="C5" s="18" t="n">
         <v>3</v>
       </c>
-      <c r="D5" s="5" t="n">
+      <c r="D5" s="18" t="n">
         <f aca="false">SUM(C4,D4)</f>
         <v>12</v>
       </c>
-      <c r="E5" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" s="13" t="s">
-        <v>50</v>
+      <c r="E5" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="20" t="s">
+        <v>94</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="45.5" outlineLevel="0" r="7">
-      <c r="B7" s="16" t="s">
-        <v>119</v>
-      </c>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
+      <c r="B7" s="24" t="s">
+        <v>122</v>
+      </c>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2637,7 +2925,7 @@
   <dimension ref="B1:H10"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="D4" activeCellId="1" pane="topLeft" sqref="D5:D13 D4"/>
+      <selection activeCell="F5" activeCellId="0" pane="topLeft" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.3"/>
@@ -2645,13 +2933,13 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.83400809716599"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.004048582996"/>
     <col collapsed="false" hidden="false" max="5" min="3" style="0" width="8.83400809716599"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="31.8623481781376"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="39.7287449392712"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.83400809716599"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="21.7" outlineLevel="0" r="1">
       <c r="B1" s="1" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="2">
@@ -2688,7 +2976,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="4">
       <c r="B4" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C4" s="5" t="n">
         <v>9</v>
@@ -2698,63 +2986,67 @@
         <v>3</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F4" s="13"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="5">
-      <c r="B5" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="C5" s="6" t="n">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="31.2" outlineLevel="0" r="5">
+      <c r="B5" s="25" t="s">
+        <v>124</v>
+      </c>
+      <c r="C5" s="26" t="n">
         <v>2</v>
       </c>
-      <c r="D5" s="5" t="n">
+      <c r="D5" s="27" t="n">
         <f aca="false">SUM(C4,D4)</f>
         <v>12</v>
       </c>
-      <c r="E5" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" s="17" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="6">
-      <c r="B6" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="C6" s="6" t="n">
+      <c r="E5" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="20" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="31.2" outlineLevel="0" r="6">
+      <c r="B6" s="25" t="s">
+        <v>126</v>
+      </c>
+      <c r="C6" s="26" t="n">
         <v>2</v>
       </c>
-      <c r="D6" s="5" t="n">
+      <c r="D6" s="27" t="n">
         <f aca="false">SUM(C5,D5)</f>
         <v>14</v>
       </c>
-      <c r="E6" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" s="17"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="7">
-      <c r="B7" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="C7" s="6" t="n">
+      <c r="E6" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="20" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="31.2" outlineLevel="0" r="7">
+      <c r="B7" s="25" t="s">
+        <v>128</v>
+      </c>
+      <c r="C7" s="26" t="n">
         <v>2</v>
       </c>
-      <c r="D7" s="5" t="n">
+      <c r="D7" s="27" t="n">
         <f aca="false">SUM(C6,D6)</f>
         <v>16</v>
       </c>
-      <c r="E7" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F7" s="17"/>
+      <c r="E7" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="20" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="8">
       <c r="B8" s="4" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="C8" s="5" t="n">
         <v>20</v>
@@ -2770,7 +3062,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="9">
       <c r="B9" s="4" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="C9" s="5" t="n">
         <v>20</v>
@@ -2783,11 +3075,11 @@
         <v>9</v>
       </c>
       <c r="F9" s="4"/>
-      <c r="H9" s="15"/>
+      <c r="H9" s="21"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="10">
       <c r="B10" s="4" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C10" s="6" t="n">
         <v>26</v>
@@ -2797,7 +3089,7 @@
         <v>58</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="F10" s="14"/>
     </row>
@@ -2820,7 +3112,7 @@
   <dimension ref="B1:F12"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="D4" activeCellId="1" pane="topLeft" sqref="D5:D13 D4"/>
+      <selection activeCell="F9" activeCellId="0" pane="topLeft" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.3"/>
@@ -2828,14 +3120,15 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.83400809716599"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.502024291498"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.83400809716599"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="9.90688259109312"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="32.1943319838057"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.35627530364373"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="7.73279352226721"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="39.9352226720648"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.83400809716599"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="21.7" outlineLevel="0" r="1">
       <c r="B1" s="1" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="2">
@@ -2872,7 +3165,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="4">
       <c r="B4" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C4" s="6" t="n">
         <v>9</v>
@@ -2882,13 +3175,13 @@
         <v>3</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F4" s="13"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="5">
       <c r="B5" s="4" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="C5" s="5" t="n">
         <v>1</v>
@@ -2898,15 +3191,15 @@
         <v>12</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="6">
       <c r="B6" s="4" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="C6" s="5" t="n">
         <v>10</v>
@@ -2920,63 +3213,63 @@
       </c>
       <c r="F6" s="4"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="7">
-      <c r="B7" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="C7" s="5" t="n">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="31.2" outlineLevel="0" r="7">
+      <c r="B7" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="C7" s="27" t="n">
         <v>2</v>
       </c>
-      <c r="D7" s="6" t="n">
+      <c r="D7" s="26" t="n">
         <f aca="false">SUM(C6,D6)</f>
         <v>23</v>
       </c>
-      <c r="E7" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F7" s="13" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="8">
-      <c r="B8" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="C8" s="5" t="n">
+      <c r="E7" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="20" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="31.2" outlineLevel="0" r="8">
+      <c r="B8" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="C8" s="27" t="n">
         <v>2</v>
       </c>
-      <c r="D8" s="6" t="n">
+      <c r="D8" s="26" t="n">
         <f aca="false">SUM(C7,D7)</f>
         <v>25</v>
       </c>
-      <c r="E8" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="F8" s="13" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="9">
-      <c r="B9" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="C9" s="5" t="n">
+      <c r="E8" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" s="20" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="31.2" outlineLevel="0" r="9">
+      <c r="B9" s="28" t="s">
+        <v>138</v>
+      </c>
+      <c r="C9" s="27" t="n">
         <v>2</v>
       </c>
-      <c r="D9" s="6" t="n">
+      <c r="D9" s="26" t="n">
         <f aca="false">SUM(C8,D8)</f>
         <v>27</v>
       </c>
-      <c r="E9" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F9" s="13" t="s">
-        <v>50</v>
+      <c r="E9" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="20" t="s">
+        <v>139</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="10">
       <c r="B10" s="4" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="C10" s="5" t="n">
         <v>20</v>
@@ -2992,7 +3285,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="11">
       <c r="B11" s="4" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
       <c r="C11" s="5" t="n">
         <v>20</v>
@@ -3008,7 +3301,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="12">
       <c r="B12" s="4" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C12" s="5" t="n">
         <v>26</v>
@@ -3018,7 +3311,7 @@
         <v>69</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="F12" s="4"/>
     </row>
@@ -3040,8 +3333,8 @@
   </sheetPr>
   <dimension ref="B2:F13"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="D5" activeCellId="0" pane="topLeft" sqref="D5:D13"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="F15" activeCellId="0" pane="topLeft" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.3"/>
@@ -3049,13 +3342,13 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.83400809716599"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26"/>
     <col collapsed="false" hidden="false" max="5" min="3" style="0" width="8.83400809716599"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="45.6113360323887"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="38.3846153846154"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.83400809716599"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="21.7" outlineLevel="0" r="2">
       <c r="B2" s="1" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="3">
@@ -3092,7 +3385,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="5">
       <c r="B5" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C5" s="5" t="n">
         <v>9</v>
@@ -3102,31 +3395,31 @@
         <v>3</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F5" s="4"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="6">
-      <c r="B6" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="C6" s="5" t="n">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="31.2" outlineLevel="0" r="6">
+      <c r="B6" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="C6" s="18" t="n">
         <v>3</v>
       </c>
-      <c r="D6" s="5" t="n">
+      <c r="D6" s="18" t="n">
         <f aca="false">SUM(C5,D5)</f>
         <v>12</v>
       </c>
-      <c r="E6" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>136</v>
+      <c r="E6" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="29" t="s">
+        <v>135</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="7">
       <c r="B7" s="4" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="C7" s="5" t="n">
         <v>200</v>
@@ -3142,7 +3435,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="8">
       <c r="B8" s="4" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="C8" s="5" t="n">
         <v>30</v>
@@ -3158,7 +3451,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="9">
       <c r="B9" s="4" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="C9" s="5" t="n">
         <v>30</v>
@@ -3174,7 +3467,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="10">
       <c r="B10" s="4" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="C10" s="5" t="n">
         <v>20</v>
@@ -3190,7 +3483,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="11">
       <c r="B11" s="4" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="C11" s="5" t="n">
         <v>20</v>
@@ -3206,7 +3499,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="12">
       <c r="B12" s="4" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C12" s="5" t="n">
         <v>26</v>
@@ -3216,26 +3509,26 @@
         <v>315</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="F12" s="4"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17" outlineLevel="0" r="13">
-      <c r="B13" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="C13" s="9" t="n">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="29.1" outlineLevel="0" r="13">
+      <c r="B13" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="C13" s="17" t="n">
         <v>20</v>
       </c>
-      <c r="D13" s="5" t="n">
+      <c r="D13" s="18" t="n">
         <f aca="false">SUM(C12,D12)</f>
         <v>341</v>
       </c>
-      <c r="E13" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>141</v>
+      <c r="E13" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="16" t="s">
+        <v>147</v>
       </c>
     </row>
   </sheetData>

</xml_diff>